<commit_message>
feat: Completed add_invoice method
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>June</t>
   </si>
@@ -23,7 +23,10 @@
     <t>EIHAB - 29 Tiff IRA</t>
   </si>
   <si>
-    <t>S K</t>
+    <t>170710-SK</t>
+  </si>
+  <si>
+    <t>EIHAB - 27 Tiff IRA</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="G22" activeCellId="0" pane="topLeft" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
@@ -419,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +547,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:32">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Add background color to cells
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="May" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="June" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>Hello World</t>
+  </si>
   <si>
     <t>June</t>
   </si>
@@ -60,12 +63,18 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF19"/>
+        <bgColor rgb="00FFFF19"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,11 +94,15 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -394,25 +407,23 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G22" activeCellId="0" pane="topLeft" sqref="G22"/>
+      <selection activeCell="H18" activeCellId="0" pane="topLeft" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="1" width="9.10526315789474"/>
+    <col customWidth="1" max="1025" min="1" style="1" width="10.6032388663968"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
-  <headerFooter differentFirst="0" differentOddEven="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -432,7 +443,7 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -532,36 +543,36 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>2</v>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Change colors from document name instead of therapist initials
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="May" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="June" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -41,6 +42,18 @@
   </si>
   <si>
     <t xml:space="preserve">Speech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIHAB - 29 Tiff IRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170710-SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIHAB - 27 Tiff IRA</t>
   </si>
 </sst>
 </file>
@@ -75,12 +88,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7C80E"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,7 +136,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,6 +149,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -139,6 +162,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFE7C80E"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -149,8 +232,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -195,4 +278,167 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AF4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9838056680162"/>
+    <col collapsed="false" hidden="false" max="32" min="2" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: Tidy up code, delete unnecessary commented out code
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" state="visible" r:id="rId2"/>
@@ -116,7 +116,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
@@ -127,13 +127,8 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>